<commit_message>
cambio de bbdd local a firebase
</commit_message>
<xml_diff>
--- a/Outfiles/Stock.xlsx
+++ b/Outfiles/Stock.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,22 +471,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>fuck</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>lets</t>
+          <t>160x130x12</t>
         </is>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -500,26 +500,26 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>cc</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>sms4</t>
+          <t>115x66x20</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>REPONER 4</t>
+          <t>SIN STOCK [5]</t>
         </is>
       </c>
     </row>
@@ -529,26 +529,26 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Valve</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>elmediavida</t>
+          <t>105x75x12</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>REPONER 3</t>
+          <t>SIN STOCK [5]</t>
         </is>
       </c>
     </row>
@@ -558,26 +558,26 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>crtl</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>control</t>
+          <t>100x80x10</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>REPONER 2</t>
+          <t>SIN STOCK [5]</t>
         </is>
       </c>
     </row>
@@ -587,26 +587,26 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>yy667</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>chaveta alfiler</t>
+          <t>100x75x10</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>REPONER 1</t>
+          <t>SIN STOCK [5]</t>
         </is>
       </c>
     </row>
@@ -616,26 +616,26 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Tesst66</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>texxt</t>
+          <t>100x62x10</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>REPONER 1</t>
+          <t>SIN STOCK [5]</t>
         </is>
       </c>
     </row>
@@ -645,26 +645,26 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Uzuu9</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ACA ESTÁ</t>
+          <t>100x60x10</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>SIN STOCK [5]</t>
         </is>
       </c>
     </row>
@@ -674,26 +674,26 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>UXU789</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>nala</t>
+          <t>95x75x10</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>SIN STOCK [5]</t>
         </is>
       </c>
     </row>
@@ -703,26 +703,26 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>de660</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>defeker</t>
+          <t>85x60x8</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>SIN STOCK [5]</t>
         </is>
       </c>
     </row>
@@ -732,26 +732,26 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>eEkaa</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>786</t>
+          <t>51,17x81 (Rojo)</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>REPONER 4</t>
         </is>
       </c>
     </row>
@@ -761,26 +761,26 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>NoOS</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>89Ba</t>
+          <t>85x58x16</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>REPONER 4</t>
         </is>
       </c>
     </row>
@@ -790,26 +790,26 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Puk88</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>paxy</t>
+          <t>85x58x10</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>REPONER 4</t>
         </is>
       </c>
     </row>
@@ -819,26 +819,26 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Eekkole</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>carta</t>
+          <t>80x55x20</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>REPONER 4</t>
         </is>
       </c>
     </row>
@@ -848,26 +848,26 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>aa55</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>galaxy 6</t>
+          <t>65x40x12 (Rojo)</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>REPONER 4</t>
         </is>
       </c>
     </row>
@@ -877,26 +877,26 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2828</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">luis </t>
+          <t>65x40x12</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>REPONER 4</t>
         </is>
       </c>
     </row>
@@ -906,26 +906,26 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Var889</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Varactor</t>
+          <t>85x65x10</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>REPONER 3</t>
         </is>
       </c>
     </row>
@@ -935,26 +935,26 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>yuuy7</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>cosa</t>
+          <t>80x48x10</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>REPONER 3</t>
         </is>
       </c>
     </row>
@@ -964,26 +964,26 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Eka99</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>bolsan</t>
+          <t>72x50x10</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>REPONER 3</t>
         </is>
       </c>
     </row>
@@ -993,26 +993,26 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>cha007</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>evelope</t>
+          <t>60x45x7</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>REPONER 3</t>
         </is>
       </c>
     </row>
@@ -1022,26 +1022,26 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Hexa99</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>hecagono</t>
+          <t>72x95x13</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>REPONER 3</t>
         </is>
       </c>
     </row>
@@ -1051,26 +1051,26 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>pd114</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>producto</t>
+          <t>55x80x10</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E22" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>REPONER 3</t>
         </is>
       </c>
     </row>
@@ -1080,26 +1080,26 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Bok88</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>juju</t>
+          <t>31.75x44.5x6.35</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>REPONER 3</t>
         </is>
       </c>
     </row>
@@ -1109,26 +1109,26 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>mouse77b6</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>mouse inalamb</t>
+          <t>62x45x10</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>REPONER 2</t>
         </is>
       </c>
     </row>
@@ -1138,26 +1138,26 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>cox88</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>nao</t>
+          <t>52x30x7</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>REPONER 2</t>
         </is>
       </c>
     </row>
@@ -1167,26 +1167,26 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Elev998</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>elevator</t>
+          <t>40x68x7</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>REPONER 2</t>
         </is>
       </c>
     </row>
@@ -1196,26 +1196,26 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>RETENLARGO7887236</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>RETEN MEDIDA LARGA 20X30X70</t>
+          <t>80x40x10</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E27" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>REPONER 1</t>
         </is>
       </c>
     </row>
@@ -1225,26 +1225,26 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Kski88</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>kusk</t>
+          <t>Sin calsif</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>REPONER 1</t>
         </is>
       </c>
     </row>
@@ -1254,26 +1254,26 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>k100</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>tellefono</t>
+          <t>68x36x10</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>REPONER 1</t>
         </is>
       </c>
     </row>
@@ -1283,26 +1283,26 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>TESTA00</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>TST</t>
+          <t>47x35x10</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E30" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>STOCK</t>
+          <t>REPONER 1</t>
         </is>
       </c>
     </row>
@@ -1312,19 +1312,19 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>pax88</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>porto</t>
+          <t>80x45x10</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
@@ -1341,19 +1341,19 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Codigo a</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Nombre Largo A</t>
+          <t>72x40x7</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
@@ -1370,19 +1370,19 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Codigo 1</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Nombre Largo 1</t>
+          <t>35x17x7</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
@@ -1399,19 +1399,19 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>upak</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>pala</t>
+          <t>60x85x8</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
@@ -1428,19 +1428,19 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Codigo b</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Nombre Largo B</t>
+          <t>90x50x10</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E35" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
@@ -1457,19 +1457,19 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Codigo 2</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Nombre Largo 2</t>
+          <t>80x50x10</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E36" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
@@ -1486,19 +1486,19 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Reten554</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Reten 30x50x60</t>
+          <t>65x85x12</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E37" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>0</v>
@@ -1515,19 +1515,19 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Codigo 3</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Nombre Largo 3</t>
+          <t>72x35x10</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="E38" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>0</v>
@@ -1544,19 +1544,19 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Codigo d</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Nombre Largo D</t>
+          <t>Sin calsif</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E39" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>0</v>
@@ -1573,19 +1573,19 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Codigo 4</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Nombre Largo 4</t>
+          <t>68x90x10</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E40" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
@@ -1602,19 +1602,19 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Codigo e</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Nombre Largo E</t>
+          <t>65x90x10</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="E41" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>0</v>
@@ -1631,19 +1631,19 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Codigo 5</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Nombre Largo 5</t>
+          <t>85x50x10</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="E42" t="n">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>0</v>
@@ -1660,19 +1660,19 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Codigo 6</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Nombre Largo 6</t>
+          <t>52x30x10</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="E43" t="n">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
@@ -1689,19 +1689,19 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Codigo 7</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Nombre Largo 7</t>
+          <t>90x70x10</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="E44" t="n">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="F44" t="n">
         <v>0</v>
@@ -1718,19 +1718,19 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Usma</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Naka</t>
+          <t>85x55x10</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
@@ -1747,19 +1747,19 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>CatOS_6.7.45</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>CatOS 6</t>
+          <t>72x45x12</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="E46" t="n">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
@@ -1776,19 +1776,19 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Codigo 8</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Nombre Largo 8</t>
+          <t>65x38x10</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="E47" t="n">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>0</v>
@@ -1805,19 +1805,19 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>CODE88</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Producto test</t>
+          <t>62x45x12</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="E48" t="n">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="F48" t="n">
         <v>0</v>
@@ -1834,19 +1834,19 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Xoda</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Soda</t>
+          <t>52x28x7</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="E49" t="n">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="F49" t="n">
         <v>0</v>
@@ -1863,19 +1863,19 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>aa123</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>alba56</t>
+          <t>52x25x7</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="E50" t="n">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>0</v>
@@ -1892,19 +1892,19 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>M&amp;M</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Rico</t>
+          <t>90x65x10</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="E51" t="n">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>0</v>
@@ -1921,19 +1921,19 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Usma</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Kamppa</t>
+          <t>72x42x10</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="E52" t="n">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>0</v>
@@ -1950,19 +1950,19 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Cul007</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Cosa</t>
+          <t>47x28x7</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="E53" t="n">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>0</v>
@@ -1979,22 +1979,22 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Vatt88</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>GVRA</t>
+          <t>47x20x7</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="E54" t="n">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2008,19 +2008,19 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>SUKA99</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>80x42x10</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
         <v>0</v>
@@ -2037,19 +2037,19 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Ursu99</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Kalolko</t>
+          <t>80x100x10</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
         <v>0</v>
@@ -2066,19 +2066,19 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Codiga778</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>nombrex</t>
+          <t>90x60x10</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="E57" t="n">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="F57" t="n">
         <v>0</v>
@@ -2095,22 +2095,22 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>5yy7</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Uxu8</t>
+          <t>80x60x10</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="E58" t="n">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="F58" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
@@ -2124,19 +2124,19 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>CatOS_5.66.7</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>CatOS 5</t>
+          <t>85x45x10</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>86</v>
+        <v>12</v>
       </c>
       <c r="E59" t="n">
-        <v>86</v>
+        <v>12</v>
       </c>
       <c r="F59" t="n">
         <v>0</v>
@@ -2153,24 +2153,53 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>ULA77700</t>
+          <t>Retén</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>CACK</t>
+          <t>72x50x10</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>567</v>
+        <v>12</v>
       </c>
       <c r="E60" t="n">
-        <v>567</v>
+        <v>12</v>
       </c>
       <c r="F60" t="n">
         <v>0</v>
       </c>
       <c r="G60" t="inlineStr">
+        <is>
+          <t>STOCK</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Retén</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>80x55x10</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>13</v>
+      </c>
+      <c r="E61" t="n">
+        <v>13</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="inlineStr">
         <is>
           <t>STOCK</t>
         </is>

</xml_diff>